<commit_message>
Update data + results
update data (2020) + results new mod (GB reviewed)
</commit_message>
<xml_diff>
--- a/results/Climatic_covariates/Climatic_trends.xlsx
+++ b/results/Climatic_covariates/Climatic_trends.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://helsinkifi-my.sharepoint.com/personal/beckeant_ad_helsinki_fi/Documents/ABS_Postdoc/Helsinki/Work/Arctic_Flowering/Zackenberg_Flowering/results/Climatic_covariates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{F5261E3E-F21C-ED4A-9084-6DCF5D565C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1888D7E2-73AA-BD44-8716-141514BB2F9D}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{F5261E3E-F21C-ED4A-9084-6DCF5D565C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03D0FE18-FC6E-4A41-BDE3-62062D1D07DF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{04FD8DCE-8CFA-2C45-8C8D-528ADE9F5520}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" activeTab="1" xr2:uid="{04FD8DCE-8CFA-2C45-8C8D-528ADE9F5520}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
-    <sheet name="Clim_year" sheetId="1" r:id="rId2"/>
-    <sheet name="Clim_season" sheetId="2" r:id="rId3"/>
+    <sheet name="Clim_season" sheetId="1" r:id="rId2"/>
+    <sheet name="Clim_year" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -881,7 +881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC775C7-65BD-9A43-B523-87AD7EABAF16}">
   <dimension ref="A2:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1043,7 +1043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DAA84B2-78D9-9D43-8ADB-9911DBEF7815}">
   <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>

</xml_diff>